<commit_message>
update codes and report issue
unable to plot spikes
</commit_message>
<xml_diff>
--- a/IntanReport_160504_Baihan.xlsx
+++ b/IntanReport_160504_Baihan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="28800" windowHeight="16460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="78">
   <si>
     <t xml:space="preserve">Report date: </t>
   </si>
@@ -32,12 +32,6 @@
     <t>Intan Analysis Report (by Baihan)</t>
   </si>
   <si>
-    <t>SpikesL</t>
-  </si>
-  <si>
-    <t>SpikesR</t>
-  </si>
-  <si>
     <t>LLEDtime</t>
   </si>
   <si>
@@ -63,13 +57,214 @@
   </si>
   <si>
     <t>RRaster</t>
+  </si>
+  <si>
+    <t>MD-011216_160112</t>
+  </si>
+  <si>
+    <t>MD-011216_contra_160112</t>
+  </si>
+  <si>
+    <t>MD-011216_contra_s2_160112</t>
+  </si>
+  <si>
+    <t>MD-011216_ipsi_160112</t>
+  </si>
+  <si>
+    <t>MD-011216_ipsi_s2__160112</t>
+  </si>
+  <si>
+    <t>MD-012516-s11_160125</t>
+  </si>
+  <si>
+    <t>MD-012516-s12_160125</t>
+  </si>
+  <si>
+    <t>MD-012516-s4_160125</t>
+  </si>
+  <si>
+    <t>MD-012516-s5_160125</t>
+  </si>
+  <si>
+    <t>MD-012516-s6_160125</t>
+  </si>
+  <si>
+    <t>MD-012516-s7_160125</t>
+  </si>
+  <si>
+    <t>MD-012516-s8_160125</t>
+  </si>
+  <si>
+    <t>/Users/DoerLBH/Dropbox/git/OLab_IntanEphys/Data//MD-012516/MD-012516-s8_160125</t>
+  </si>
+  <si>
+    <t>MD-012516-s9_160125</t>
+  </si>
+  <si>
+    <t>/Users/DoerLBH/Dropbox/git/OLab_IntanEphys/Data//MD-012516/MD-012516-s9_160125</t>
+  </si>
+  <si>
+    <t>MD-012516_160125</t>
+  </si>
+  <si>
+    <t>Ctrl-012616-S10_160126</t>
+  </si>
+  <si>
+    <t>Ctrl-012616-S11_160126</t>
+  </si>
+  <si>
+    <t>Ctrl-012616-S3_160126</t>
+  </si>
+  <si>
+    <t>/Users/DoerLBH/Dropbox/git/OLab_IntanEphys/Data//Normal-012616/Ctrl-012616-S3_160126</t>
+  </si>
+  <si>
+    <t>Ctrl-012616-S4_160126</t>
+  </si>
+  <si>
+    <t>Ctrl-012616-S5_160126</t>
+  </si>
+  <si>
+    <t>Ctrl-012616-S6_160126</t>
+  </si>
+  <si>
+    <t>/Users/DoerLBH/Dropbox/git/OLab_IntanEphys/Data//Normal-012616/Ctrl-012616-S6_160126</t>
+  </si>
+  <si>
+    <t>Ctrl-012616-S7_160126</t>
+  </si>
+  <si>
+    <t>Ctrl-012616-S8_160126</t>
+  </si>
+  <si>
+    <t>/Users/DoerLBH/Dropbox/git/OLab_IntanEphys/Data//Normal-012616/Ctrl-012616-S8_160126</t>
+  </si>
+  <si>
+    <t>Ctrl-012616-S9_160126</t>
+  </si>
+  <si>
+    <t>albino-012816-S10_160128</t>
+  </si>
+  <si>
+    <t>albino-012816-S11_160128</t>
+  </si>
+  <si>
+    <t>albino-012816-S12_160128</t>
+  </si>
+  <si>
+    <t>albino-012816-S13_160128</t>
+  </si>
+  <si>
+    <t>albino-012816-S14_160128</t>
+  </si>
+  <si>
+    <t>albino-012816-S15_160128</t>
+  </si>
+  <si>
+    <t>/Users/DoerLBH/Dropbox/git/OLab_IntanEphys/Data//albino-012816/albino-012816-S15_160128</t>
+  </si>
+  <si>
+    <t>albino-012816-S1_160128</t>
+  </si>
+  <si>
+    <t>albino-012816-S3_160128</t>
+  </si>
+  <si>
+    <t>/Users/DoerLBH/Dropbox/git/OLab_IntanEphys/Data//albino-012816/albino-012816-S3_160128</t>
+  </si>
+  <si>
+    <t>albino-012816-S4_160128</t>
+  </si>
+  <si>
+    <t>/Users/DoerLBH/Dropbox/git/OLab_IntanEphys/Data//albino-012816/albino-012816-S4_160128</t>
+  </si>
+  <si>
+    <t>albino-012816-S5_160128</t>
+  </si>
+  <si>
+    <t>albino-012816-S6_160128</t>
+  </si>
+  <si>
+    <t>albino-012816-S7_160128</t>
+  </si>
+  <si>
+    <t>/Users/DoerLBH/Dropbox/git/OLab_IntanEphys/Data//albino-012816/albino-012816-S7_160128</t>
+  </si>
+  <si>
+    <t>albino-012816-S8_160128</t>
+  </si>
+  <si>
+    <t>albino-012816-S9_160128</t>
+  </si>
+  <si>
+    <t>albino-020116-S10_160201</t>
+  </si>
+  <si>
+    <t>/Users/DoerLBH/Dropbox/git/OLab_IntanEphys/Data//albino-020116/albino-020116-S10_160201</t>
+  </si>
+  <si>
+    <t>albino-020116-S11_160201</t>
+  </si>
+  <si>
+    <t>albino-020116-S12_160201</t>
+  </si>
+  <si>
+    <t>/Users/DoerLBH/Dropbox/git/OLab_IntanEphys/Data//albino-020116/albino-020116-S12_160201</t>
+  </si>
+  <si>
+    <t>albino-020116-S1_160201</t>
+  </si>
+  <si>
+    <t>albino-020116-S3_160201</t>
+  </si>
+  <si>
+    <t>/Users/DoerLBH/Dropbox/git/OLab_IntanEphys/Data//albino-020116/albino-020116-S3_160201</t>
+  </si>
+  <si>
+    <t>albino-020116-S4_160201</t>
+  </si>
+  <si>
+    <t>albino-020116-S5_160201</t>
+  </si>
+  <si>
+    <t>/Users/DoerLBH/Dropbox/git/OLab_IntanEphys/Data//albino-020116/albino-020116-S5_160201</t>
+  </si>
+  <si>
+    <t>albino-020116-S6_160201</t>
+  </si>
+  <si>
+    <t>albino-020116-S7_160201</t>
+  </si>
+  <si>
+    <t>albino-020116-S8_160201</t>
+  </si>
+  <si>
+    <t>albino-020116-S9_160201</t>
+  </si>
+  <si>
+    <t>WARNING!_Failed_to_detect_LED!</t>
+  </si>
+  <si>
+    <t>Fail_to_record_all?</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Case</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Done </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -92,6 +287,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="DengXian"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -126,7 +327,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -137,6 +338,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -416,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:N87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -427,12 +634,12 @@
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="37" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" ht="37" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -440,40 +647,1043 @@
         <v>42494</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="4" t="s">
+    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="E5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="F5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="G5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="H5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="I5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="J5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="K5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="1" t="s">
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="4"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" s="7"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="C8" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B9" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="C9" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="4">
+        <v>14</v>
+      </c>
+      <c r="E13" s="4">
+        <v>6</v>
+      </c>
+      <c r="F13" s="4">
+        <v>81</v>
+      </c>
+      <c r="G13" s="4">
+        <v>78.5</v>
+      </c>
+      <c r="H13" s="4">
+        <v>87.166700000000006</v>
+      </c>
+      <c r="I13" s="4">
+        <v>89.166700000000006</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="4">
+        <v>27</v>
+      </c>
+      <c r="E14" s="4">
+        <v>16</v>
+      </c>
+      <c r="F14" s="4">
+        <v>124.5926</v>
+      </c>
+      <c r="G14" s="4">
+        <v>118.2593</v>
+      </c>
+      <c r="H14" s="4">
+        <v>120.5625</v>
+      </c>
+      <c r="I14" s="4">
+        <v>119.6875</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="4">
+        <v>6</v>
+      </c>
+      <c r="E18" s="4">
+        <v>9</v>
+      </c>
+      <c r="F18" s="4">
+        <v>109.83329999999999</v>
+      </c>
+      <c r="G18" s="4">
+        <v>126.66670000000001</v>
+      </c>
+      <c r="H18" s="4">
+        <v>150.4444</v>
+      </c>
+      <c r="I18" s="4">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B19" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B20" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J20" s="4"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B22" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="4">
+        <v>1</v>
+      </c>
+      <c r="E22" s="4">
+        <v>2</v>
+      </c>
+      <c r="F22" s="4">
+        <v>15</v>
+      </c>
+      <c r="G22" s="4">
+        <v>43</v>
+      </c>
+      <c r="H22" s="4">
+        <v>107</v>
+      </c>
+      <c r="I22" s="4">
+        <v>102.5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="4">
+        <v>11</v>
+      </c>
+      <c r="E23" s="4">
+        <v>2</v>
+      </c>
+      <c r="F23" s="4">
+        <v>73.090900000000005</v>
+      </c>
+      <c r="G23" s="4">
+        <v>70</v>
+      </c>
+      <c r="H23" s="4">
+        <v>40</v>
+      </c>
+      <c r="I23" s="4">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B24" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B25" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B26" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B27" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B28" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J28" s="4"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B29" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J29" s="4"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B30" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="4">
+        <v>2</v>
+      </c>
+      <c r="E30" s="4">
+        <v>3</v>
+      </c>
+      <c r="F30" s="4">
+        <v>26</v>
+      </c>
+      <c r="G30" s="4">
+        <v>36.5</v>
+      </c>
+      <c r="H30" s="4">
+        <v>95</v>
+      </c>
+      <c r="I30" s="4">
+        <v>40.666699999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B31" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D31" s="4">
+        <v>1</v>
+      </c>
+      <c r="E31" s="4">
+        <v>4</v>
+      </c>
+      <c r="F31" s="4">
+        <v>79</v>
+      </c>
+      <c r="G31" s="4">
+        <v>25</v>
+      </c>
+      <c r="H31" s="4">
+        <v>62</v>
+      </c>
+      <c r="I31" s="4">
+        <v>94.25</v>
+      </c>
+      <c r="J31" s="4"/>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B32" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J32" s="4"/>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B33" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D33" s="4">
+        <v>2</v>
+      </c>
+      <c r="E33" s="4">
+        <v>1</v>
+      </c>
+      <c r="F33" s="4">
+        <v>55.5</v>
+      </c>
+      <c r="G33" s="4">
+        <v>60.5</v>
+      </c>
+      <c r="H33" s="4">
+        <v>1</v>
+      </c>
+      <c r="I33" s="4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B34" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D34" s="4">
+        <v>5</v>
+      </c>
+      <c r="E34" s="4">
+        <v>5</v>
+      </c>
+      <c r="F34" s="4">
+        <v>11.2</v>
+      </c>
+      <c r="G34" s="4">
+        <v>41</v>
+      </c>
+      <c r="H34" s="4">
+        <v>36.6</v>
+      </c>
+      <c r="I34" s="4">
+        <v>33.6</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B35" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B36" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B37" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B38" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J38" s="4"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B39" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J39" s="4"/>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B40" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D40" s="4">
+        <v>7</v>
+      </c>
+      <c r="E40" s="4">
+        <v>2</v>
+      </c>
+      <c r="F40" s="4">
+        <v>58.142899999999997</v>
+      </c>
+      <c r="G40" s="4">
+        <v>46</v>
+      </c>
+      <c r="H40" s="4">
+        <v>53</v>
+      </c>
+      <c r="I40" s="4">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B41" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D41" s="4">
+        <v>3</v>
+      </c>
+      <c r="E41" s="4">
+        <v>8</v>
+      </c>
+      <c r="F41" s="4">
+        <v>12</v>
+      </c>
+      <c r="G41" s="4">
+        <v>66.666700000000006</v>
+      </c>
+      <c r="H41" s="4">
+        <v>34.625</v>
+      </c>
+      <c r="I41" s="4">
+        <v>25.625</v>
+      </c>
+      <c r="J41" s="4"/>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B42" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J42" s="4"/>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B43" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D43" s="4">
+        <v>1</v>
+      </c>
+      <c r="E43" s="4">
+        <v>1</v>
+      </c>
+      <c r="F43" s="4">
+        <v>98</v>
+      </c>
+      <c r="G43" s="4">
+        <v>7</v>
+      </c>
+      <c r="H43" s="4">
+        <v>19</v>
+      </c>
+      <c r="I43" s="4">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B44" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D44" s="4">
+        <v>4</v>
+      </c>
+      <c r="E44" s="4">
+        <v>4</v>
+      </c>
+      <c r="F44" s="4">
+        <v>32.5</v>
+      </c>
+      <c r="G44" s="4">
+        <v>11.75</v>
+      </c>
+      <c r="H44" s="4">
+        <v>15</v>
+      </c>
+      <c r="I44" s="4">
+        <v>15.5</v>
+      </c>
+      <c r="J44" s="4"/>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B45" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B46" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D46" s="4">
+        <v>4</v>
+      </c>
+      <c r="E46" s="4">
+        <v>2</v>
+      </c>
+      <c r="F46" s="4">
+        <v>52.5</v>
+      </c>
+      <c r="G46" s="4">
+        <v>87.5</v>
+      </c>
+      <c r="H46" s="4">
+        <v>5</v>
+      </c>
+      <c r="I46" s="4">
+        <v>45.5</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B47" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B48" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J48" s="4"/>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B49" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B50" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D50" s="4">
+        <v>1</v>
+      </c>
+      <c r="E50" s="4">
+        <v>4</v>
+      </c>
+      <c r="F50" s="4">
+        <v>4</v>
+      </c>
+      <c r="G50" s="4">
+        <v>4</v>
+      </c>
+      <c r="H50" s="4">
+        <v>8.5</v>
+      </c>
+      <c r="I50" s="4">
+        <v>16.5</v>
+      </c>
+      <c r="J50" s="4"/>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B51" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J51" s="4"/>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B52" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D52" s="4">
+        <v>7</v>
+      </c>
+      <c r="E52" s="4">
+        <v>5</v>
+      </c>
+      <c r="F52" s="4">
+        <v>11.428599999999999</v>
+      </c>
+      <c r="G52" s="4">
+        <v>10.571400000000001</v>
+      </c>
+      <c r="H52" s="4">
+        <v>9.4</v>
+      </c>
+      <c r="I52" s="4">
+        <v>11.2</v>
+      </c>
+      <c r="J52" s="4"/>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B53" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D53" s="4">
+        <v>6</v>
+      </c>
+      <c r="E53" s="4">
+        <v>1</v>
+      </c>
+      <c r="F53" s="4">
+        <v>20.5</v>
+      </c>
+      <c r="G53" s="4">
+        <v>31</v>
+      </c>
+      <c r="H53" s="4">
+        <v>17</v>
+      </c>
+      <c r="I53" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B54" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D54" s="4">
+        <v>1</v>
+      </c>
+      <c r="E54" s="4">
+        <v>4</v>
+      </c>
+      <c r="F54" s="4">
+        <v>54</v>
+      </c>
+      <c r="G54" s="4">
+        <v>80</v>
+      </c>
+      <c r="H54" s="4">
+        <v>9.25</v>
+      </c>
+      <c r="I54" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B55" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B56" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B58" s="4"/>
+    </row>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="4"/>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B60" s="4"/>
+    </row>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="4"/>
+      <c r="E61" s="4"/>
+    </row>
+    <row r="62" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B62" s="4"/>
+    </row>
+    <row r="63" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
+      <c r="G63" s="4"/>
+      <c r="H63" s="4"/>
+      <c r="I63" s="4"/>
+    </row>
+    <row r="64" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B64" s="4"/>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B65" s="4"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
+      <c r="G65" s="4"/>
+      <c r="H65" s="4"/>
+      <c r="I65" s="4"/>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B66" s="4"/>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4"/>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B68" s="4"/>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B69" s="4"/>
+      <c r="C69" s="4"/>
+      <c r="D69" s="4"/>
+      <c r="E69" s="4"/>
+      <c r="F69" s="4"/>
+      <c r="G69" s="4"/>
+      <c r="H69" s="4"/>
+      <c r="I69" s="4"/>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B70" s="4"/>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B71" s="4"/>
+      <c r="C71" s="4"/>
+      <c r="D71" s="4"/>
+      <c r="E71" s="4"/>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B72" s="4"/>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B73" s="4"/>
+      <c r="C73" s="4"/>
+      <c r="D73" s="4"/>
+    </row>
+    <row r="74" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B74" s="4"/>
+      <c r="C74" s="4"/>
+      <c r="D74" s="4"/>
+      <c r="E74" s="4"/>
+    </row>
+    <row r="75" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B75" s="4"/>
+    </row>
+    <row r="76" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B76" s="4"/>
+      <c r="C76" s="4"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="4"/>
+      <c r="G76" s="4"/>
+      <c r="H76" s="4"/>
+      <c r="I76" s="4"/>
+    </row>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B77" s="4"/>
+    </row>
+    <row r="78" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B78" s="4"/>
+      <c r="C78" s="4"/>
+      <c r="D78" s="4"/>
+      <c r="E78" s="4"/>
+    </row>
+    <row r="79" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B79" s="4"/>
+    </row>
+    <row r="80" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B80" s="4"/>
+      <c r="C80" s="4"/>
+      <c r="D80" s="4"/>
+      <c r="E80" s="4"/>
+      <c r="F80" s="4"/>
+      <c r="G80" s="4"/>
+      <c r="H80" s="4"/>
+      <c r="I80" s="4"/>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B81" s="4"/>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B82" s="4"/>
+      <c r="C82" s="4"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="4"/>
+      <c r="F82" s="4"/>
+      <c r="G82" s="4"/>
+      <c r="H82" s="4"/>
+      <c r="I82" s="4"/>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B83" s="4"/>
+    </row>
+    <row r="84" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B84" s="4"/>
+      <c r="C84" s="4"/>
+      <c r="D84" s="4"/>
+      <c r="E84" s="4"/>
+      <c r="F84" s="4"/>
+      <c r="G84" s="4"/>
+      <c r="H84" s="4"/>
+      <c r="I84" s="4"/>
+    </row>
+    <row r="85" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B85" s="4"/>
+    </row>
+    <row r="86" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B86" s="4"/>
+      <c r="C86" s="4"/>
+      <c r="D86" s="4"/>
+    </row>
+    <row r="87" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B87" s="4"/>
+      <c r="C87" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>